<commit_message>
read data from multiple sheets and merge
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Staffs" sheetId="1" r:id="rId1"/>
-    <sheet name="SalaryLevel" sheetId="2" r:id="rId2"/>
+    <sheet name="Staffs_2015" sheetId="3" r:id="rId2"/>
+    <sheet name="SalaryLevel" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +89,18 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>bill@gmail.com</t>
+  </si>
+  <si>
+    <t>ben@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -164,9 +177,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,7 +464,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,65 +477,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -587,9 +600,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>65</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>234</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>